<commit_message>
Update lesson 29 DataProvider and Excel
</commit_message>
<xml_diff>
--- a/datatest/Login.xlsx
+++ b/datatest/Login.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ANHTESTER\SeleniumJava\Course_Selenium_Java_4_2022\SeleniumMaven42022Parallel\datatest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5104F3C5-35BC-4EAF-9BAC-DFAE2F6D56F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{558C9F67-A3CC-4D4A-BC15-78E3B9BE2120}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2400" yWindow="1056" windowWidth="18600" windowHeight="11184" xr2:uid="{EE356032-7105-40D1-9155-08C684D97174}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="9">
   <si>
     <t>username</t>
   </si>
@@ -52,6 +52,15 @@
   </si>
   <si>
     <t>cedric.kelly</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>role</t>
   </si>
 </sst>
 </file>
@@ -102,11 +111,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -421,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89038B6D-F0E0-4300-897E-29EC2E9B7C44}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -434,7 +444,7 @@
     <col min="3" max="3" width="14.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -444,29 +454,113 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update lesson 31 Test Listener TestNG
</commit_message>
<xml_diff>
--- a/datatest/Login.xlsx
+++ b/datatest/Login.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ANHTESTER\SeleniumJava\Course_Selenium_Java_4_2022\SeleniumMaven42022Parallel\datatest\"/>
     </mc:Choice>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="12">
   <si>
     <t>username</t>
   </si>
@@ -61,12 +61,22 @@
   </si>
   <si>
     <t>role</t>
+  </si>
+  <si>
+    <t>passed</t>
+  </si>
+  <si>
+    <t>success</t>
+  </si>
+  <si>
+    <t>failed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="14"/>
@@ -85,7 +95,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -96,6 +106,36 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="57"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="57"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
       </patternFill>
     </fill>
   </fills>
@@ -111,12 +151,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -439,9 +488,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" customWidth="1"/>
-    <col min="2" max="2" width="16.58203125" customWidth="1"/>
-    <col min="3" max="3" width="14.25" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="14.6640625"/>
+    <col min="2" max="2" customWidth="true" width="16.58203125"/>
+    <col min="3" max="3" customWidth="true" width="14.25"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
@@ -485,8 +534,8 @@
       <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>6</v>
+      <c r="C3" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>6</v>
@@ -502,8 +551,8 @@
       <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>6</v>
+      <c r="C4" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>6</v>
@@ -519,8 +568,8 @@
       <c r="B5" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>6</v>
+      <c r="C5" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Update lesson 33 - Extent Report Allure Report
</commit_message>
<xml_diff>
--- a/datatest/Login.xlsx
+++ b/datatest/Login.xlsx
@@ -3,21 +3,21 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ANHTESTER\SeleniumJava\Course_Selenium_Java_4_2022\SeleniumMaven42022Parallel\datatest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{558C9F67-A3CC-4D4A-BC15-78E3B9BE2120}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44A738DD-3D6E-4678-BF2E-915E42C2D798}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2400" yWindow="1056" windowWidth="18600" windowHeight="11184" xr2:uid="{EE356032-7105-40D1-9155-08C684D97174}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{EE356032-7105-40D1-9155-08C684D97174}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="12">
   <si>
     <t>username</t>
   </si>
@@ -76,7 +76,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="14"/>
@@ -95,7 +94,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -109,28 +108,13 @@
       </patternFill>
     </fill>
     <fill>
-      <patternFill patternType="none">
+      <patternFill patternType="solid">
         <fgColor indexed="57"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="57"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
         <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="10"/>
       </patternFill>
     </fill>
     <fill>
@@ -157,13 +141,13 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -483,14 +467,14 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="14.6640625"/>
-    <col min="2" max="2" customWidth="true" width="16.58203125"/>
-    <col min="3" max="3" customWidth="true" width="14.25"/>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="16.58203125" customWidth="1"/>
+    <col min="3" max="3" width="14.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Update ConstantGlobal.java and configs.properties
</commit_message>
<xml_diff>
--- a/datatest/Login.xlsx
+++ b/datatest/Login.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ANHTESTER\SeleniumJava\Course_Selenium_Java_4_2022\SeleniumMaven42022Parallel\datatest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44A738DD-3D6E-4678-BF2E-915E42C2D798}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{014EE75D-7E22-4BDE-9FF6-733FD2114DC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{EE356032-7105-40D1-9155-08C684D97174}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="9">
   <si>
     <t>username</t>
   </si>
@@ -61,15 +61,6 @@
   </si>
   <si>
     <t>role</t>
-  </si>
-  <si>
-    <t>passed</t>
-  </si>
-  <si>
-    <t>success</t>
-  </si>
-  <si>
-    <t>failed</t>
   </si>
 </sst>
 </file>
@@ -94,7 +85,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -105,21 +96,6 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="57"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
       </patternFill>
     </fill>
   </fills>
@@ -135,19 +111,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -467,7 +438,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -501,9 +472,7 @@
       <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="C2" s="3"/>
       <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
@@ -518,9 +487,7 @@
       <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>9</v>
-      </c>
+      <c r="C3" s="4"/>
       <c r="D3" s="2" t="s">
         <v>6</v>
       </c>
@@ -535,9 +502,7 @@
       <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>10</v>
-      </c>
+      <c r="C4" s="4"/>
       <c r="D4" s="2" t="s">
         <v>6</v>
       </c>
@@ -552,9 +517,7 @@
       <c r="B5" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>11</v>
-      </c>
+      <c r="C5" s="4"/>
       <c r="D5" s="2" t="s">
         <v>6</v>
       </c>
@@ -569,9 +532,7 @@
       <c r="B6" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="C6" s="3"/>
       <c r="D6" s="2" t="s">
         <v>6</v>
       </c>
@@ -586,9 +547,7 @@
       <c r="B7" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="C7" s="3"/>
       <c r="D7" s="2" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
Update Selenium 4.12.1 and HRM system
</commit_message>
<xml_diff>
--- a/datatest/Login.xlsx
+++ b/datatest/Login.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ANHTESTER\SeleniumJava\Course_Selenium_Java_4_2022\SeleniumMaven42022Parallel\datatest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ANHTESTER\SeleniumJava\Course_SeleniumJava_042022\SeleniumMaven42022Parallel\datatest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{014EE75D-7E22-4BDE-9FF6-733FD2114DC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3D9CD9B-BFF8-480F-BFCC-E4490D418F1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{EE356032-7105-40D1-9155-08C684D97174}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{EE356032-7105-40D1-9155-08C684D97174}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="11">
   <si>
     <t>username</t>
   </si>
@@ -61,6 +61,12 @@
   </si>
   <si>
     <t>role</t>
+  </si>
+  <si>
+    <t>admin_example</t>
+  </si>
+  <si>
+    <t>project_manager</t>
   </si>
 </sst>
 </file>
@@ -71,7 +77,7 @@
     <font>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
@@ -80,7 +86,7 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -111,14 +117,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -438,17 +443,17 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" customWidth="1"/>
-    <col min="2" max="2" width="16.58203125" customWidth="1"/>
-    <col min="3" max="3" width="14.25" customWidth="1"/>
+    <col min="1" max="1" width="14.69140625" customWidth="1"/>
+    <col min="2" max="2" width="16.61328125" customWidth="1"/>
+    <col min="3" max="3" width="14.23046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -465,14 +470,14 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="3"/>
+        <v>9</v>
+      </c>
+      <c r="B2">
+        <v>123456</v>
+      </c>
+      <c r="C2" s="2"/>
       <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
@@ -480,14 +485,14 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="4"/>
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>123456</v>
+      </c>
+      <c r="C3" s="3"/>
       <c r="D3" s="2" t="s">
         <v>6</v>
       </c>
@@ -495,14 +500,14 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="4"/>
+      <c r="C4" s="3"/>
       <c r="D4" s="2" t="s">
         <v>6</v>
       </c>
@@ -510,14 +515,14 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="4"/>
+      <c r="C5" s="3"/>
       <c r="D5" s="2" t="s">
         <v>6</v>
       </c>
@@ -525,14 +530,14 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="3"/>
+      <c r="C6" s="2"/>
       <c r="D6" s="2" t="s">
         <v>6</v>
       </c>
@@ -540,14 +545,14 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="3"/>
+      <c r="C7" s="2"/>
       <c r="D7" s="2" t="s">
         <v>6</v>
       </c>

</xml_diff>